<commit_message>
servlet 5 6 7
</commit_message>
<xml_diff>
--- a/DayWiseContent.xlsx
+++ b/DayWiseContent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JFST124\Day3\FirstRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F589656-1CC8-47CA-97DC-F4C6BA8124EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212309C0-17CB-4B2A-92B1-14CC48CE02ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D04D2797-0940-44A3-AF0A-8BCE4B9779F6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="240">
   <si>
     <t>Day1</t>
   </si>
@@ -812,6 +812,15 @@
   </si>
   <si>
     <t>Download and configure Tomcat Server</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>doGet and doPost</t>
+  </si>
+  <si>
+    <t>casestudy</t>
   </si>
 </sst>
 </file>
@@ -1234,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A50B4F-F5E0-4E59-AF30-46E2CF7E1AC0}">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1889,6 +1898,21 @@
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D95" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D98" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>